<commit_message>
Almost done implementing MAP referencing
</commit_message>
<xml_diff>
--- a/Grades/Design Review 1 Grades.xlsx
+++ b/Grades/Design Review 1 Grades.xlsx
@@ -5,18 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emh203\Documents\GitHub\Flux-Capacitors\Grades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calvin HP\Desktop\Flux-Capacitors\Grades\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34730" windowHeight="17820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34725" windowHeight="17820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -274,23 +271,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Summary"/>
-      <sheetName val="Participation"/>
-      <sheetName val="DR 1- RAS JAM"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,18 +539,18 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="109.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="109.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -598,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -632,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
@@ -692,7 +672,7 @@
         <v>86.875</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -748,7 +728,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
@@ -804,7 +784,7 @@
         <v>8.875</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
@@ -860,7 +840,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -916,7 +896,7 @@
         <v>8.875</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
@@ -972,7 +952,7 @@
         <v>8.4375</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>17</v>
       </c>
@@ -1028,7 +1008,7 @@
         <v>8.1875</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>18</v>
       </c>
@@ -1084,7 +1064,7 @@
         <v>9.1875</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
@@ -1140,7 +1120,7 @@
         <v>9.1875</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>20</v>
       </c>
@@ -1196,7 +1176,7 @@
         <v>8.1875</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>

</xml_diff>